<commit_message>
Block Ctrl + A/X/V, added abs/rel coordinates to Event
</commit_message>
<xml_diff>
--- a/Indexes.xlsx
+++ b/Indexes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Виталий\source\work_repos\TextComponent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80444037-0F89-4B91-A182-2FE30138E262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E7D787-5AF8-418C-BE16-9AA23E046F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ACF5A844-2569-4FB9-AF6A-F7B2E0297C9D}"/>
   </bookViews>
@@ -116,7 +116,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +135,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -148,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,6 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -473,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394D4A61-97E2-4DF0-819B-B280B04E54B2}">
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AC6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5:AC5"/>
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,6 +853,95 @@
         <v>28</v>
       </c>
     </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4">
+        <v>25</v>
+      </c>
+      <c r="D6" s="4">
+        <v>26</v>
+      </c>
+      <c r="E6" s="4">
+        <v>27</v>
+      </c>
+      <c r="F6" s="4">
+        <v>28</v>
+      </c>
+      <c r="G6" s="4">
+        <v>29</v>
+      </c>
+      <c r="H6" s="4">
+        <v>30</v>
+      </c>
+      <c r="I6" s="4">
+        <v>31</v>
+      </c>
+      <c r="J6" s="4">
+        <v>32</v>
+      </c>
+      <c r="K6" s="4">
+        <v>33</v>
+      </c>
+      <c r="L6" s="4">
+        <v>34</v>
+      </c>
+      <c r="M6" s="4">
+        <v>35</v>
+      </c>
+      <c r="N6" s="4">
+        <v>36</v>
+      </c>
+      <c r="O6" s="4">
+        <v>37</v>
+      </c>
+      <c r="P6" s="4">
+        <v>38</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>39</v>
+      </c>
+      <c r="R6" s="4">
+        <v>40</v>
+      </c>
+      <c r="S6" s="4">
+        <v>41</v>
+      </c>
+      <c r="T6" s="4">
+        <v>42</v>
+      </c>
+      <c r="U6" s="4">
+        <v>43</v>
+      </c>
+      <c r="V6" s="4">
+        <v>44</v>
+      </c>
+      <c r="W6" s="4">
+        <v>45</v>
+      </c>
+      <c r="X6" s="4">
+        <v>46</v>
+      </c>
+      <c r="Y6" s="4">
+        <v>47</v>
+      </c>
+      <c r="Z6" s="4">
+        <v>48</v>
+      </c>
+      <c r="AA6" s="4">
+        <v>49</v>
+      </c>
+      <c r="AB6" s="4">
+        <v>50</v>
+      </c>
+      <c r="AC6" s="4">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed OutOfRange Error when two lines is empty, new selection format (Start, Length, Line) in Event
</commit_message>
<xml_diff>
--- a/Indexes.xlsx
+++ b/Indexes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Виталий\source\work_repos\TextComponent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E7D787-5AF8-418C-BE16-9AA23E046F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8E1940-20CF-4095-887A-6126CB90F4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ACF5A844-2569-4FB9-AF6A-F7B2E0297C9D}"/>
   </bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A1:AC6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <selection activeCell="U4" sqref="U4:AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed line number error when splitter character is at zero position
</commit_message>
<xml_diff>
--- a/Indexes.xlsx
+++ b/Indexes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Виталий\source\work_repos\TextComponent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8E1940-20CF-4095-887A-6126CB90F4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09083179-E089-434D-B515-611E467288E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ACF5A844-2569-4FB9-AF6A-F7B2E0297C9D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="31">
   <si>
     <t>Д</t>
   </si>
@@ -100,6 +100,33 @@
   </si>
   <si>
     <t>г</t>
+  </si>
+  <si>
+    <t>Т</t>
+  </si>
+  <si>
+    <t>у</t>
+  </si>
+  <si>
+    <t>Е</t>
+  </si>
+  <si>
+    <t>щ</t>
+  </si>
+  <si>
+    <t>ё</t>
+  </si>
+  <si>
+    <t>ь</t>
+  </si>
+  <si>
+    <t>ш</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -116,7 +143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +168,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -154,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,6 +199,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -480,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394D4A61-97E2-4DF0-819B-B280B04E54B2}">
-  <dimension ref="A1:AC6"/>
+  <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4:AC4"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,7 +553,7 @@
     <col min="29" max="29" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -585,7 +620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -656,7 +691,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -681,7 +716,7 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -764,7 +799,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>0</v>
       </c>
@@ -853,7 +888,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>23</v>
       </c>
@@ -940,6 +975,833 @@
       </c>
       <c r="AC6" s="4">
         <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="X9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>0</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+      <c r="D10" s="6">
+        <v>3</v>
+      </c>
+      <c r="E10" s="6">
+        <v>4</v>
+      </c>
+      <c r="F10" s="6">
+        <v>5</v>
+      </c>
+      <c r="G10" s="6">
+        <v>6</v>
+      </c>
+      <c r="H10" s="6">
+        <v>7</v>
+      </c>
+      <c r="I10" s="6">
+        <v>8</v>
+      </c>
+      <c r="J10" s="6">
+        <v>9</v>
+      </c>
+      <c r="K10" s="6">
+        <v>10</v>
+      </c>
+      <c r="L10" s="6">
+        <v>11</v>
+      </c>
+      <c r="M10" s="6">
+        <v>12</v>
+      </c>
+      <c r="N10" s="6">
+        <v>13</v>
+      </c>
+      <c r="O10" s="6">
+        <v>14</v>
+      </c>
+      <c r="P10" s="6">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>16</v>
+      </c>
+      <c r="R10" s="6">
+        <v>17</v>
+      </c>
+      <c r="S10" s="6">
+        <v>18</v>
+      </c>
+      <c r="T10" s="6">
+        <v>19</v>
+      </c>
+      <c r="U10" s="6">
+        <v>20</v>
+      </c>
+      <c r="V10" s="6">
+        <v>21</v>
+      </c>
+      <c r="W10" s="6">
+        <v>22</v>
+      </c>
+      <c r="X10" s="6">
+        <v>23</v>
+      </c>
+      <c r="Y10" s="6">
+        <v>24</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>25</v>
+      </c>
+      <c r="AA10" s="6">
+        <v>26</v>
+      </c>
+      <c r="AB10" s="6">
+        <v>27</v>
+      </c>
+      <c r="AC10" s="6">
+        <v>28</v>
+      </c>
+      <c r="AD10" s="6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>0</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2</v>
+      </c>
+      <c r="D13" s="6">
+        <v>3</v>
+      </c>
+      <c r="E13" s="6">
+        <v>4</v>
+      </c>
+      <c r="F13" s="6">
+        <v>5</v>
+      </c>
+      <c r="G13" s="6">
+        <v>6</v>
+      </c>
+      <c r="H13" s="6">
+        <v>7</v>
+      </c>
+      <c r="I13" s="6">
+        <v>8</v>
+      </c>
+      <c r="J13" s="6">
+        <v>9</v>
+      </c>
+      <c r="K13" s="6">
+        <v>10</v>
+      </c>
+      <c r="L13" s="6">
+        <v>11</v>
+      </c>
+      <c r="M13" s="6">
+        <v>12</v>
+      </c>
+      <c r="N13" s="6">
+        <v>13</v>
+      </c>
+      <c r="O13" s="6">
+        <v>14</v>
+      </c>
+      <c r="P13" s="6">
+        <v>15</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>16</v>
+      </c>
+      <c r="R13" s="6">
+        <v>17</v>
+      </c>
+      <c r="S13" s="6">
+        <v>18</v>
+      </c>
+      <c r="T13" s="6">
+        <v>19</v>
+      </c>
+      <c r="U13" s="6">
+        <v>20</v>
+      </c>
+      <c r="V13" s="6">
+        <v>21</v>
+      </c>
+      <c r="W13" s="6">
+        <v>22</v>
+      </c>
+      <c r="X13" s="6">
+        <v>23</v>
+      </c>
+      <c r="Y13" s="6">
+        <v>24</v>
+      </c>
+      <c r="Z13" s="6">
+        <v>25</v>
+      </c>
+      <c r="AA13" s="6">
+        <v>26</v>
+      </c>
+      <c r="AB13" s="6">
+        <v>27</v>
+      </c>
+      <c r="AC13" s="6">
+        <v>28</v>
+      </c>
+      <c r="AD13" s="6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>30</v>
+      </c>
+      <c r="B14" s="4">
+        <v>31</v>
+      </c>
+      <c r="C14" s="4">
+        <v>32</v>
+      </c>
+      <c r="D14" s="4">
+        <v>33</v>
+      </c>
+      <c r="E14" s="4">
+        <v>34</v>
+      </c>
+      <c r="F14" s="4">
+        <v>35</v>
+      </c>
+      <c r="G14" s="4">
+        <v>36</v>
+      </c>
+      <c r="H14" s="4">
+        <v>37</v>
+      </c>
+      <c r="I14" s="4">
+        <v>38</v>
+      </c>
+      <c r="J14" s="4">
+        <v>39</v>
+      </c>
+      <c r="K14" s="4">
+        <v>40</v>
+      </c>
+      <c r="L14" s="4">
+        <v>41</v>
+      </c>
+      <c r="M14" s="4">
+        <v>42</v>
+      </c>
+      <c r="N14" s="4">
+        <v>43</v>
+      </c>
+      <c r="O14" s="4">
+        <v>44</v>
+      </c>
+      <c r="P14" s="4">
+        <v>45</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>46</v>
+      </c>
+      <c r="R14" s="4">
+        <v>47</v>
+      </c>
+      <c r="S14" s="4">
+        <v>48</v>
+      </c>
+      <c r="T14" s="4">
+        <v>49</v>
+      </c>
+      <c r="U14" s="4">
+        <v>50</v>
+      </c>
+      <c r="V14" s="4">
+        <v>51</v>
+      </c>
+      <c r="W14" s="4">
+        <v>52</v>
+      </c>
+      <c r="X14" s="4">
+        <v>53</v>
+      </c>
+      <c r="Y14" s="4">
+        <v>54</v>
+      </c>
+      <c r="Z14" s="4">
+        <v>55</v>
+      </c>
+      <c r="AA14" s="4">
+        <v>56</v>
+      </c>
+      <c r="AB14" s="4">
+        <v>57</v>
+      </c>
+      <c r="AC14" s="4">
+        <v>58</v>
+      </c>
+      <c r="AD14" s="4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="R16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>0</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2</v>
+      </c>
+      <c r="D17" s="6">
+        <v>3</v>
+      </c>
+      <c r="E17" s="6">
+        <v>4</v>
+      </c>
+      <c r="F17" s="6">
+        <v>5</v>
+      </c>
+      <c r="G17" s="6">
+        <v>6</v>
+      </c>
+      <c r="H17" s="6">
+        <v>7</v>
+      </c>
+      <c r="I17" s="6">
+        <v>8</v>
+      </c>
+      <c r="J17" s="6">
+        <v>9</v>
+      </c>
+      <c r="K17" s="6">
+        <v>10</v>
+      </c>
+      <c r="L17" s="6">
+        <v>11</v>
+      </c>
+      <c r="M17" s="6">
+        <v>12</v>
+      </c>
+      <c r="N17" s="6">
+        <v>13</v>
+      </c>
+      <c r="O17" s="6">
+        <v>14</v>
+      </c>
+      <c r="P17" s="6">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>16</v>
+      </c>
+      <c r="R17" s="6">
+        <v>17</v>
+      </c>
+      <c r="S17" s="6">
+        <v>18</v>
+      </c>
+      <c r="T17" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>60</v>
+      </c>
+      <c r="B18" s="4">
+        <v>61</v>
+      </c>
+      <c r="C18" s="4">
+        <v>62</v>
+      </c>
+      <c r="D18" s="4">
+        <v>63</v>
+      </c>
+      <c r="E18" s="4">
+        <v>64</v>
+      </c>
+      <c r="F18" s="4">
+        <v>65</v>
+      </c>
+      <c r="G18" s="4">
+        <v>66</v>
+      </c>
+      <c r="H18" s="4">
+        <v>67</v>
+      </c>
+      <c r="I18" s="4">
+        <v>68</v>
+      </c>
+      <c r="J18" s="4">
+        <v>69</v>
+      </c>
+      <c r="K18" s="4">
+        <v>70</v>
+      </c>
+      <c r="L18" s="4">
+        <v>71</v>
+      </c>
+      <c r="M18" s="4">
+        <v>72</v>
+      </c>
+      <c r="N18" s="4">
+        <v>73</v>
+      </c>
+      <c r="O18" s="4">
+        <v>74</v>
+      </c>
+      <c r="P18" s="4">
+        <v>75</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>76</v>
+      </c>
+      <c r="R18" s="4">
+        <v>77</v>
+      </c>
+      <c r="S18" s="4">
+        <v>78</v>
+      </c>
+      <c r="T18" s="4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="R24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T24" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>0</v>
+      </c>
+      <c r="B25" s="6">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6">
+        <v>2</v>
+      </c>
+      <c r="D25" s="6">
+        <v>3</v>
+      </c>
+      <c r="E25" s="6">
+        <v>4</v>
+      </c>
+      <c r="F25" s="6">
+        <v>5</v>
+      </c>
+      <c r="G25" s="6">
+        <v>6</v>
+      </c>
+      <c r="H25" s="6">
+        <v>7</v>
+      </c>
+      <c r="I25" s="6">
+        <v>8</v>
+      </c>
+      <c r="J25" s="6">
+        <v>9</v>
+      </c>
+      <c r="K25" s="6">
+        <v>10</v>
+      </c>
+      <c r="L25" s="6">
+        <v>11</v>
+      </c>
+      <c r="M25" s="6">
+        <v>12</v>
+      </c>
+      <c r="N25" s="6">
+        <v>13</v>
+      </c>
+      <c r="O25" s="6">
+        <v>14</v>
+      </c>
+      <c r="P25" s="6">
+        <v>15</v>
+      </c>
+      <c r="Q25" s="6">
+        <v>16</v>
+      </c>
+      <c r="R25" s="6">
+        <v>17</v>
+      </c>
+      <c r="S25" s="6">
+        <v>18</v>
+      </c>
+      <c r="T25" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>81</v>
+      </c>
+      <c r="B26" s="4">
+        <v>82</v>
+      </c>
+      <c r="C26" s="4">
+        <v>83</v>
+      </c>
+      <c r="D26" s="4">
+        <v>84</v>
+      </c>
+      <c r="E26" s="4">
+        <v>85</v>
+      </c>
+      <c r="F26" s="4">
+        <v>86</v>
+      </c>
+      <c r="G26" s="4">
+        <v>87</v>
+      </c>
+      <c r="H26" s="4">
+        <v>88</v>
+      </c>
+      <c r="I26" s="4">
+        <v>89</v>
+      </c>
+      <c r="J26" s="4">
+        <v>90</v>
+      </c>
+      <c r="K26" s="4">
+        <v>91</v>
+      </c>
+      <c r="L26" s="4">
+        <v>92</v>
+      </c>
+      <c r="M26" s="4">
+        <v>93</v>
+      </c>
+      <c r="N26" s="4">
+        <v>94</v>
+      </c>
+      <c r="O26" s="4">
+        <v>95</v>
+      </c>
+      <c r="P26" s="4">
+        <v>96</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>97</v>
+      </c>
+      <c r="R26" s="4">
+        <v>98</v>
+      </c>
+      <c r="S26" s="4">
+        <v>99</v>
+      </c>
+      <c r="T26" s="4">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>